<commit_message>
Updated grades for homework 3
</commit_message>
<xml_diff>
--- a/Fundamentals_workshop_2023/Other/FOR_workshop_grading_sheet.xlsx
+++ b/Fundamentals_workshop_2023/Other/FOR_workshop_grading_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/henriquesposito/Documents/GitHub/Fundamentals_of_R_IHEID2022/Fundamentals_workshop_2023/Other/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9387E58C-6FD9-2C4F-A827-2140AC494967}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE8CAE86-31BB-404B-907E-D7F4D2D2C48D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2200" yWindow="1320" windowWidth="28040" windowHeight="16520" xr2:uid="{95C89197-D342-644B-A96F-2085E8F4C3FA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="67">
   <si>
     <t>Name</t>
   </si>
@@ -134,9 +134,6 @@
     <t>Varun Paresh Vithalani</t>
   </si>
   <si>
-    <t>Did not submit the homework until 17/3/2023 at 9 am…</t>
-  </si>
-  <si>
     <t>Gisenly Garcias Garcia</t>
   </si>
   <si>
@@ -185,9 +182,6 @@
     <t>very good attempt, did all on his own</t>
   </si>
   <si>
-    <t>no submission by 8:45</t>
-  </si>
-  <si>
     <t>came to office hours, a bit of an unorganized script</t>
   </si>
   <si>
@@ -201,6 +195,48 @@
   </si>
   <si>
     <t>Submitted the data, not an R script, was not able to open… submitted 10 days after**</t>
+  </si>
+  <si>
+    <t>Did not submit the homework until 17/3/2023 at 9 am… Sumitted late, stopped at number 5</t>
+  </si>
+  <si>
+    <t>Homework 3</t>
+  </si>
+  <si>
+    <t>no submission by 8:45… submitted late and stopped at question 6 (codes do not run after)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no submission by 8:45 … submitted late, using codes that we did not teach in base R… ** </t>
+  </si>
+  <si>
+    <t>Great, submitted a knitted PDF all correct but could have made plots prettier with labs…</t>
+  </si>
+  <si>
+    <t>Submitted an Rmd doc that knits to html, came to OH, plots were good</t>
+  </si>
+  <si>
+    <t>Submitted an Rmd doc that does not knit (data is missing), but the rest is good</t>
+  </si>
+  <si>
+    <t>Great, all is correct!</t>
+  </si>
+  <si>
+    <t>Tried and made a few mistakes with plotting, but everything is good.</t>
+  </si>
+  <si>
+    <t>submitted an r script, all seems correct but not an RMD</t>
+  </si>
+  <si>
+    <t>Good attempt, got a few plots wrong but overall good!</t>
+  </si>
+  <si>
+    <t>Missing question 6, rest is ok</t>
+  </si>
+  <si>
+    <t>Great attempt, a few very minor issues but did all on his own!</t>
+  </si>
+  <si>
+    <t>Submited and Rmd file, stopped at 5, plots were not the nicest</t>
   </si>
 </sst>
 </file>
@@ -552,10 +588,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA2DBCDA-AC56-3347-B3C6-9DC99A32046A}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -563,10 +599,11 @@
     <col min="1" max="1" width="38" customWidth="1"/>
     <col min="2" max="2" width="71.5" customWidth="1"/>
     <col min="3" max="3" width="30.5" customWidth="1"/>
-    <col min="4" max="4" width="33" customWidth="1"/>
+    <col min="4" max="4" width="50.1640625" customWidth="1"/>
+    <col min="6" max="6" width="39.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -577,13 +614,19 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -594,13 +637,19 @@
         <v>5.25</v>
       </c>
       <c r="D2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E2">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2">
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -611,13 +660,19 @@
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E3">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G3">
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -628,13 +683,19 @@
         <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E4">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -645,13 +706,19 @@
         <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E5">
         <v>5.75</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G5">
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -662,13 +729,19 @@
         <v>5.75</v>
       </c>
       <c r="D6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E6">
         <v>5.75</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F6" t="s">
+        <v>59</v>
+      </c>
+      <c r="G6">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -679,13 +752,19 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E7">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F7" t="s">
+        <v>60</v>
+      </c>
+      <c r="G7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -696,13 +775,19 @@
         <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E8">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F8" t="s">
+        <v>57</v>
+      </c>
+      <c r="G8">
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -713,13 +798,19 @@
         <v>5.5</v>
       </c>
       <c r="D9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E9">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F9" t="s">
+        <v>61</v>
+      </c>
+      <c r="G9">
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -730,13 +821,19 @@
         <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E10">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F10" t="s">
+        <v>60</v>
+      </c>
+      <c r="G10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -747,13 +844,19 @@
         <v>5.5</v>
       </c>
       <c r="D11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E11">
         <v>5.5</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F11" t="s">
+        <v>62</v>
+      </c>
+      <c r="G11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -764,13 +867,19 @@
         <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E12">
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F12" t="s">
+        <v>60</v>
+      </c>
+      <c r="G12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -781,27 +890,42 @@
         <v>5.5</v>
       </c>
       <c r="D13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E13">
         <v>6</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F13" t="s">
+        <v>63</v>
+      </c>
+      <c r="G13">
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C14">
         <v>5.5</v>
       </c>
       <c r="D14" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+        <v>56</v>
+      </c>
+      <c r="E14">
+        <v>5</v>
+      </c>
+      <c r="F14" t="s">
+        <v>64</v>
+      </c>
+      <c r="G14">
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -812,13 +936,19 @@
         <v>5.25</v>
       </c>
       <c r="D15" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E15">
         <v>6</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F15" t="s">
+        <v>57</v>
+      </c>
+      <c r="G15">
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -829,13 +959,19 @@
         <v>5</v>
       </c>
       <c r="D16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E16">
         <v>6</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F16" t="s">
+        <v>60</v>
+      </c>
+      <c r="G16">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -846,13 +982,19 @@
         <v>6</v>
       </c>
       <c r="D17" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E17">
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F17" t="s">
+        <v>65</v>
+      </c>
+      <c r="G17">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -863,13 +1005,19 @@
         <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E18">
         <v>5.5</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F18" t="s">
+        <v>63</v>
+      </c>
+      <c r="G18">
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -880,40 +1028,61 @@
         <v>5.5</v>
       </c>
       <c r="D19" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E19">
         <v>6</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F19" t="s">
+        <v>58</v>
+      </c>
+      <c r="G19">
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>31</v>
       </c>
       <c r="B20" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20">
+        <v>4.5</v>
+      </c>
+      <c r="D20" t="s">
+        <v>55</v>
+      </c>
+      <c r="E20">
+        <v>4</v>
+      </c>
+      <c r="F20" t="s">
+        <v>66</v>
+      </c>
+      <c r="G20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>32</v>
       </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
-      <c r="D20" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="B21" t="s">
         <v>33</v>
-      </c>
-      <c r="B21" t="s">
-        <v>34</v>
       </c>
       <c r="C21">
         <v>5.25</v>
       </c>
       <c r="D21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E21">
+        <v>6</v>
+      </c>
+      <c r="F21" t="s">
+        <v>43</v>
+      </c>
+      <c r="G21">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Graded homework 1 for this workshop. Different sheet in the same excel file.
</commit_message>
<xml_diff>
--- a/Fundamentals_workshop_2023/Other/FOR_workshop_grading_sheet.xlsx
+++ b/Fundamentals_workshop_2023/Other/FOR_workshop_grading_sheet.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/henriquesposito/Documents/GitHub/Fundamentals_of_R_IHEID2022/Fundamentals_workshop_2023/Other/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE8CAE86-31BB-404B-907E-D7F4D2D2C48D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{126B1F9B-5C8C-3444-9785-3D17883263CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2200" yWindow="1320" windowWidth="28040" windowHeight="16520" xr2:uid="{95C89197-D342-644B-A96F-2085E8F4C3FA}"/>
+    <workbookView xWindow="2200" yWindow="1320" windowWidth="28040" windowHeight="16520" activeTab="1" xr2:uid="{95C89197-D342-644B-A96F-2085E8F4C3FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="89">
   <si>
     <t>Name</t>
   </si>
@@ -237,6 +238,72 @@
   </si>
   <si>
     <t>Submited and Rmd file, stopped at 5, plots were not the nicest</t>
+  </si>
+  <si>
+    <t>Chanbormey Ouk</t>
+  </si>
+  <si>
+    <t>Clara Zuccarino</t>
+  </si>
+  <si>
+    <t>Emma Guitera</t>
+  </si>
+  <si>
+    <t>Good effort but some answers were incorrect…</t>
+  </si>
+  <si>
+    <t>Esteban Filippa-Ocampo</t>
+  </si>
+  <si>
+    <t>Good job (only unable to do bonus question). Next time please comment answers</t>
+  </si>
+  <si>
+    <t>Good job (only unable to do bonus question)</t>
+  </si>
+  <si>
+    <t>Ishankaur Khalsa</t>
+  </si>
+  <si>
+    <t>Jane Wilkinson</t>
+  </si>
+  <si>
+    <t>Good effort, some answers were incorrect but attempted the bonus question</t>
+  </si>
+  <si>
+    <t>Kevin Alejandro Gomez Anguiano</t>
+  </si>
+  <si>
+    <t>Luciana Markstein</t>
+  </si>
+  <si>
+    <t>Great job, even did bonus question!</t>
+  </si>
+  <si>
+    <t>Paniz Jamali</t>
+  </si>
+  <si>
+    <t>Sent us a PHG file…</t>
+  </si>
+  <si>
+    <t>Samia Firmino Pinto</t>
+  </si>
+  <si>
+    <t>Good effort, not the most straighforard way to do some things but most answers were correct!</t>
+  </si>
+  <si>
+    <t>Sebastian Zünd</t>
+  </si>
+  <si>
+    <t>Willow Sylvester</t>
+  </si>
+  <si>
+    <t>Xinyu Liu</t>
+  </si>
+  <si>
+    <t>Yixin Du</t>
+  </si>
+  <si>
+    <t>Nameetta Nierakkal</t>
   </si>
 </sst>
 </file>
@@ -590,8 +657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA2DBCDA-AC56-3347-B3C6-9DC99A32046A}">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B1" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1089,4 +1156,209 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17D99A16-6F37-9A46-AF31-01DE287A5AE0}">
+  <dimension ref="A1:G16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="31.83203125" customWidth="1"/>
+    <col min="2" max="2" width="80.83203125" customWidth="1"/>
+    <col min="3" max="3" width="8.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7">
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>78</v>
+      </c>
+      <c r="B9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>82</v>
+      </c>
+      <c r="B11" t="s">
+        <v>83</v>
+      </c>
+      <c r="C11">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>84</v>
+      </c>
+      <c r="B12" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>85</v>
+      </c>
+      <c r="B13" t="s">
+        <v>79</v>
+      </c>
+      <c r="C13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>86</v>
+      </c>
+      <c r="B14" t="s">
+        <v>76</v>
+      </c>
+      <c r="C14">
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>87</v>
+      </c>
+      <c r="B15" t="s">
+        <v>76</v>
+      </c>
+      <c r="C15">
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>88</v>
+      </c>
+      <c r="B16" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16">
+        <v>5.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Graded assignments and updated practical
</commit_message>
<xml_diff>
--- a/Fundamentals_workshop_2023/Other/FOR_workshop_grading_sheet.xlsx
+++ b/Fundamentals_workshop_2023/Other/FOR_workshop_grading_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/henriquesposito/Documents/GitHub/Fundamentals_of_R_IHEID2022/Fundamentals_workshop_2023/Other/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFBE44C6-6044-AB40-B048-9D93D7BE8E88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11444E32-F83A-0A4D-9586-334D5D1C3633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2200" yWindow="1320" windowWidth="28040" windowHeight="16520" activeTab="1" xr2:uid="{95C89197-D342-644B-A96F-2085E8F4C3FA}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="102">
   <si>
     <t>Name</t>
   </si>
@@ -321,7 +321,28 @@
     <t>Ruizi Yu</t>
   </si>
   <si>
-    <t>No submission - late</t>
+    <t>Good job! Next time please comment answers</t>
+  </si>
+  <si>
+    <t>Great job!</t>
+  </si>
+  <si>
+    <t>Good job! Unable to do a few using R but left everything commented</t>
+  </si>
+  <si>
+    <t>Good job! Updated 2 files but all seems ok</t>
+  </si>
+  <si>
+    <t>Sent us an assignment with 3 questions only?</t>
+  </si>
+  <si>
+    <t>Good job! Not the most efficient code but got things done</t>
+  </si>
+  <si>
+    <t>No submission - No justification</t>
+  </si>
+  <si>
+    <t>Asked for an extension beforehand…</t>
   </si>
 </sst>
 </file>
@@ -1181,7 +1202,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1189,6 +1210,7 @@
     <col min="1" max="1" width="31.83203125" customWidth="1"/>
     <col min="2" max="2" width="80.83203125" customWidth="1"/>
     <col min="3" max="3" width="8.1640625" customWidth="1"/>
+    <col min="4" max="4" width="61.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -1224,6 +1246,12 @@
       <c r="C2">
         <v>6</v>
       </c>
+      <c r="D2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E2">
+        <v>6</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -1235,6 +1263,12 @@
       <c r="C3">
         <v>6</v>
       </c>
+      <c r="D3" t="s">
+        <v>95</v>
+      </c>
+      <c r="E3">
+        <v>6</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -1246,6 +1280,12 @@
       <c r="C4">
         <v>5.5</v>
       </c>
+      <c r="D4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E4">
+        <v>6</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -1257,6 +1297,12 @@
       <c r="C5">
         <v>6</v>
       </c>
+      <c r="D5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E5">
+        <v>5.75</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -1268,6 +1314,12 @@
       <c r="C6">
         <v>6</v>
       </c>
+      <c r="D6" t="s">
+        <v>97</v>
+      </c>
+      <c r="E6">
+        <v>6</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -1279,6 +1331,12 @@
       <c r="C7">
         <v>5.75</v>
       </c>
+      <c r="D7" t="s">
+        <v>95</v>
+      </c>
+      <c r="E7">
+        <v>6</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -1290,6 +1348,9 @@
       <c r="C8">
         <v>6</v>
       </c>
+      <c r="D8" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -1301,6 +1362,12 @@
       <c r="C9">
         <v>6</v>
       </c>
+      <c r="D9" t="s">
+        <v>95</v>
+      </c>
+      <c r="E9">
+        <v>6</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -1309,6 +1376,12 @@
       <c r="B10" t="s">
         <v>81</v>
       </c>
+      <c r="D10" t="s">
+        <v>98</v>
+      </c>
+      <c r="E10">
+        <v>3</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -1320,6 +1393,12 @@
       <c r="C11">
         <v>5.5</v>
       </c>
+      <c r="D11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E11">
+        <v>6</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -1331,6 +1410,12 @@
       <c r="C12">
         <v>6</v>
       </c>
+      <c r="D12" t="s">
+        <v>95</v>
+      </c>
+      <c r="E12">
+        <v>6</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -1342,6 +1427,12 @@
       <c r="C13">
         <v>6</v>
       </c>
+      <c r="D13" t="s">
+        <v>99</v>
+      </c>
+      <c r="E13">
+        <v>6</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -1353,6 +1444,12 @@
       <c r="C14">
         <v>5.75</v>
       </c>
+      <c r="D14" t="s">
+        <v>95</v>
+      </c>
+      <c r="E14">
+        <v>6</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
@@ -1364,6 +1461,12 @@
       <c r="C15">
         <v>5.75</v>
       </c>
+      <c r="D15" t="s">
+        <v>95</v>
+      </c>
+      <c r="E15">
+        <v>6</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
@@ -1375,59 +1478,95 @@
       <c r="C16">
         <v>5.5</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D16" t="s">
+        <v>101</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>89</v>
       </c>
       <c r="B17" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="C17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D17" t="s">
+        <v>100</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>90</v>
       </c>
       <c r="B18" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="C18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D18" t="s">
+        <v>100</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>91</v>
       </c>
       <c r="B19" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="C19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D19" t="s">
+        <v>100</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>92</v>
       </c>
       <c r="B20" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="C20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D20" t="s">
+        <v>100</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>93</v>
       </c>
       <c r="B21" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21" t="s">
+        <v>100</v>
+      </c>
+      <c r="E21">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added final grades to grading sheet
</commit_message>
<xml_diff>
--- a/Fundamentals_workshop_2023/Other/FOR_workshop_grading_sheet.xlsx
+++ b/Fundamentals_workshop_2023/Other/FOR_workshop_grading_sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/henriquesposito/Documents/GitHub/Fundamentals_of_R_IHEID2022/Fundamentals_workshop_2023/Other/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{478B5307-81AD-3B4F-BD6F-55E8A723787C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{670EC64B-4E81-F748-8CF7-EB0AE6346B2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2200" yWindow="1320" windowWidth="28040" windowHeight="16520" activeTab="1" xr2:uid="{95C89197-D342-644B-A96F-2085E8F4C3FA}"/>
+    <workbookView xWindow="2200" yWindow="1320" windowWidth="28040" windowHeight="16520" xr2:uid="{95C89197-D342-644B-A96F-2085E8F4C3FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -421,7 +421,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -440,6 +440,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -453,10 +459,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -773,8 +780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA2DBCDA-AC56-3347-B3C6-9DC99A32046A}">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -787,548 +794,548 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="2" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
         <v>5.25</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E2">
-        <v>6</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="E2" s="2">
+        <v>6</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="2">
         <v>5.75</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="2" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2">
         <v>5</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E3">
-        <v>6</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="E3" s="2">
+        <v>6</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="2">
         <v>5.75</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="2" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C4">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="C4" s="2">
+        <v>6</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E4">
-        <v>6</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="E4" s="2">
+        <v>6</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="G4">
-        <v>6</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="G4" s="2">
+        <v>6</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C5">
-        <v>6</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="C5" s="2">
+        <v>6</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="2">
         <v>5.75</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="2">
         <v>5.75</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="2" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="2">
         <v>5.75</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="2">
         <v>5.75</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="2">
         <v>5.5</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="2" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C7">
-        <v>6</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="C7" s="2">
+        <v>6</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E7">
-        <v>6</v>
-      </c>
-      <c r="F7" t="s">
+      <c r="E7" s="2">
+        <v>6</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="G7">
-        <v>6</v>
-      </c>
-      <c r="H7" t="s">
+      <c r="G7" s="2">
+        <v>6</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C8">
-        <v>6</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="C8" s="2">
+        <v>6</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E8">
-        <v>6</v>
-      </c>
-      <c r="F8" t="s">
+      <c r="E8" s="2">
+        <v>6</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="2">
         <v>5.75</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="2" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="2">
         <v>5.5</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E9">
-        <v>6</v>
-      </c>
-      <c r="F9" t="s">
+      <c r="E9" s="2">
+        <v>6</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="2">
         <v>5.75</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="2" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="A10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C10">
-        <v>6</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="C10" s="2">
+        <v>6</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E10">
-        <v>6</v>
-      </c>
-      <c r="F10" t="s">
+      <c r="E10" s="2">
+        <v>6</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="G10">
-        <v>6</v>
-      </c>
-      <c r="H10" t="s">
+      <c r="G10" s="2">
+        <v>6</v>
+      </c>
+      <c r="H10" s="2" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="2">
         <v>5.5</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="2">
         <v>5.5</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="2">
         <v>5</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11" s="2" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="A12" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C12">
-        <v>6</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="C12" s="2">
+        <v>6</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E12">
-        <v>6</v>
-      </c>
-      <c r="F12" t="s">
+      <c r="E12" s="2">
+        <v>6</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="G12">
-        <v>6</v>
-      </c>
-      <c r="H12" t="s">
+      <c r="G12" s="2">
+        <v>6</v>
+      </c>
+      <c r="H12" s="2" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="A13" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="2">
         <v>5.5</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E13">
-        <v>6</v>
-      </c>
-      <c r="F13" t="s">
+      <c r="E13" s="2">
+        <v>6</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="2">
         <v>5.75</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H13" s="2" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="A14" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="2">
         <v>5.5</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="2">
         <v>5</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="2">
         <v>5.75</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H14" s="2" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="A15" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="2">
         <v>5.25</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E15">
-        <v>6</v>
-      </c>
-      <c r="F15" t="s">
+      <c r="E15" s="2">
+        <v>6</v>
+      </c>
+      <c r="F15" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="2">
         <v>5.75</v>
       </c>
-      <c r="H15" t="s">
+      <c r="H15" s="2" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="A16" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="2">
         <v>5</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E16">
-        <v>6</v>
-      </c>
-      <c r="F16" t="s">
+      <c r="E16" s="2">
+        <v>6</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="G16">
-        <v>6</v>
-      </c>
-      <c r="H16" t="s">
+      <c r="G16" s="2">
+        <v>6</v>
+      </c>
+      <c r="H16" s="2" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="A17" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C17">
-        <v>6</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="C17" s="2">
+        <v>6</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E17">
-        <v>6</v>
-      </c>
-      <c r="F17" t="s">
+      <c r="E17" s="2">
+        <v>6</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="G17">
-        <v>6</v>
-      </c>
-      <c r="H17" t="s">
+      <c r="G17" s="2">
+        <v>6</v>
+      </c>
+      <c r="H17" s="2" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="A18" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="2">
         <v>5</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="2">
         <v>5.5</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="2">
         <v>5.75</v>
       </c>
-      <c r="H18" t="s">
+      <c r="H18" s="2" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="A19" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="2">
         <v>5.5</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E19">
-        <v>6</v>
-      </c>
-      <c r="F19" t="s">
+      <c r="E19" s="2">
+        <v>6</v>
+      </c>
+      <c r="F19" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="2">
         <v>5.75</v>
       </c>
-      <c r="H19" t="s">
+      <c r="H19" s="2" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="A20" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="2">
         <v>4.5</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="2">
         <v>4</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="2">
         <v>5</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H20" s="2" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="A21" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="2">
         <v>5.25</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E21">
-        <v>6</v>
-      </c>
-      <c r="F21" t="s">
+      <c r="E21" s="2">
+        <v>6</v>
+      </c>
+      <c r="F21" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="G21">
-        <v>6</v>
-      </c>
-      <c r="H21" t="s">
+      <c r="G21" s="2">
+        <v>6</v>
+      </c>
+      <c r="H21" s="2" t="s">
         <v>117</v>
       </c>
     </row>
@@ -1341,8 +1348,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17D99A16-6F37-9A46-AF31-01DE287A5AE0}">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1504,7 +1511,7 @@
       <c r="F6" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="3">
         <v>0</v>
       </c>
       <c r="H6" s="2" t="s">
@@ -1770,7 +1777,7 @@
       <c r="F16" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="G16" s="2">
+      <c r="G16" s="3">
         <v>0</v>
       </c>
       <c r="H16" s="2" t="s">

</xml_diff>